<commit_message>
fix Athlete outcome trimester fetus_weight_t == decimal
</commit_message>
<xml_diff>
--- a/dictionaries/outcome_ath/1_0/1_0_trimester_rep.xlsx
+++ b/dictionaries/outcome_ath/1_0/1_0_trimester_rep.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\back\ATHLETE\HARMO\20220613_dicts\fetal\forGithub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FD57D5-15B7-43FD-B708-D1411C04063E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F58DBB-E190-47A7-B088-215D2D9775BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="32760" windowWidth="16380" windowHeight="8190" tabRatio="256" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32760" yWindow="32760" windowWidth="16380" windowHeight="8190" tabRatio="256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="2" r:id="rId1"/>
@@ -1245,8 +1245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1398,7 +1398,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
         <v>36</v>
@@ -1606,8 +1606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Athlete outcome_ath trimester ga_us_t == decimal
</commit_message>
<xml_diff>
--- a/dictionaries/outcome_ath/1_0/1_0_trimester_rep.xlsx
+++ b/dictionaries/outcome_ath/1_0/1_0_trimester_rep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\back\ATHLETE\HARMO\20220613_dicts\fetal\forGithub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F58DBB-E190-47A7-B088-215D2D9775BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC7A22D-4744-4054-9B47-F3E4A52B0B38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32760" yWindow="32760" windowWidth="16380" windowHeight="8190" tabRatio="256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1246,7 +1246,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1328,7 +1328,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
         <v>33</v>

</xml_diff>